<commit_message>
add: se mapea id para su visualizacion en Excel
</commit_message>
<xml_diff>
--- a/src/exports/empresas_categoria_food.xlsx.xlsx
+++ b/src/exports/empresas_categoria_food.xlsx.xlsx
@@ -430,26 +430,29 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="str">
+        <v>67bf38f0a9c0f101fb8c8295</v>
+      </c>
       <c r="B2" t="str">
-        <v>campero</v>
+        <v>Pollo Grangero</v>
       </c>
       <c r="C2" t="str">
-        <v>Medium</v>
+        <v>Medio</v>
       </c>
       <c r="D2">
-        <v>1971</v>
+        <v>2010</v>
       </c>
       <c r="E2" t="str">
         <v>Food</v>
       </c>
       <c r="F2" t="str">
-        <v>Empresa dedicada a la venta de Pollos y más.</v>
+        <v>Empresa de comida.</v>
       </c>
       <c r="G2" s="1">
         <v>45714.41199854167</v>
       </c>
       <c r="H2" s="1">
-        <v>45714.41199854167</v>
+        <v>45714.430585925926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>